<commit_message>
neues Dokument für Doku & Vervollständigen der Excel
</commit_message>
<xml_diff>
--- a/Meetings/Doku/Struktur_Doku - 2015.10.12 - EinkaufsApp Übersicht bis dato - AK HD TE.xlsx
+++ b/Meetings/Doku/Struktur_Doku - 2015.10.12 - EinkaufsApp Übersicht bis dato - AK HD TE.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dang\Desktop\EinkaufsApp\EinkaufsApp-Doku\Meetings\Doku\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="6135"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="6135" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Skilltabelle" sheetId="9" r:id="rId1"/>
@@ -25,12 +20,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Telkos, Besprechungstermine'!$A$1:$C$1</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="161">
   <si>
     <t>Datum</t>
   </si>
@@ -1720,12 +1715,42 @@
   <si>
     <t>Durchfühungsphase</t>
   </si>
+  <si>
+    <t>Michael Ausarbeitung</t>
+  </si>
+  <si>
+    <t>Micha Benutzerverwaltung:
+Aufgabe: Erstellen einer Benutzerverwaltung
+Tools: MongoDB, Robomongo
+Runtime Environment: NodeJS
+Sprache: JavaScript
+Funktion der Verwaltung:
+- Registrieren 
+        - Test ob Benutzername/Email bereits vergeben sind
+        - Test ob Email wirklich das Format einer Email hat
+        - Test ob die Passwörter übereinstimmen --&gt; das Passwort wird als Hash in der  Datenbank gespeichert
+- Login/ Logout
+        - Test ob Benutzername/Passwort korrekt
+- Passwort vergessen 
+        - Sendet Email hinterlegte Mail mit einem Token im Link welches nur eine Stunde gültig ist
+        - Token ist für Passwort zurücksetzen 
+ --&gt; Fehler wenn die Email nicht in der DB existiert welches nur eine Stunde gültig ist
+- Passwort zurücksetzen
+        - Überprüfung ob die Passwörter übereinstimmen
+- Funktion zum schützen von Routen
+        - kann in jede Route via „require“ eingebunden und genutzt werden
+        - verhindert, dass man eine Route ohne ein Login sehen kann
+        - Diese Anfrage wird auf die Login Seite weitergeleitet</t>
+  </si>
+  <si>
+    <t>Durchführungsphase</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1783,6 +1808,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1853,7 +1885,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1970,9 +2002,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1989,9 +2026,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2029,9 +2066,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2066,7 +2103,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2101,7 +2138,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2277,7 +2314,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -2863,13 +2900,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2956,8 +2993,95 @@
         <v>114</v>
       </c>
     </row>
+    <row r="6" spans="1:6" ht="360" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
+        <v>42288</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C6" s="52" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="50"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="50"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="51"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="50"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="50"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="50"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="50"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C14" s="50"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C15" s="50"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="50"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="50"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="50"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="50"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="50"/>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="50"/>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="50"/>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="50"/>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="50"/>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="50"/>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="50"/>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="50"/>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="50"/>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="50"/>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="50"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update Skillliste, Gruppenaufteilung, Ablaufplan
</commit_message>
<xml_diff>
--- a/Meetings/Doku/Struktur_Doku - 2015.10.12 - EinkaufsApp Übersicht bis dato - AK HD TE.xlsx
+++ b/Meetings/Doku/Struktur_Doku - 2015.10.12 - EinkaufsApp Übersicht bis dato - AK HD TE.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dang\Desktop\EinkaufsApp\EinkaufsApp-Doku\Meetings\Doku\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="6135" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="6135" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Skilltabelle" sheetId="9" r:id="rId1"/>
@@ -12,20 +17,27 @@
     <sheet name="Design" sheetId="1" r:id="rId3"/>
     <sheet name="Dev" sheetId="2" r:id="rId4"/>
     <sheet name="Doku" sheetId="7" r:id="rId5"/>
-    <sheet name="genutzte Links" sheetId="8" r:id="rId6"/>
-    <sheet name="Tools" sheetId="4" r:id="rId7"/>
-    <sheet name="Telkos, Besprechungstermine" sheetId="5" r:id="rId8"/>
-    <sheet name="Zusatzinfos" sheetId="6" r:id="rId9"/>
+    <sheet name="Ablaufplan" sheetId="10" r:id="rId6"/>
+    <sheet name="Gruppenaufteilung" sheetId="11" r:id="rId7"/>
+    <sheet name="genutzte Links" sheetId="8" r:id="rId8"/>
+    <sheet name="Tools" sheetId="4" r:id="rId9"/>
+    <sheet name="Telkos, Besprechungstermine" sheetId="5" r:id="rId10"/>
+    <sheet name="Zusatzinfos" sheetId="6" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Telkos, Besprechungstermine'!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Ablaufplan!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">alle!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Design!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Dev!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Gruppenaufteilung!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Telkos, Besprechungstermine'!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="249">
   <si>
     <t>Datum</t>
   </si>
@@ -1745,12 +1757,301 @@
   <si>
     <t>Durchführungsphase</t>
   </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">*Änderung Gruppenaufteilung (Daniel ist jetzt bei den Designern!)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*ToDos bis 30.10.15: Skilliste, Abstimmung GS1, einzelne Tätigkeiten in der Gruppe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+*Ablaufplan (s. Reiter "Ablaufplan"), nicht fix</t>
+    </r>
+  </si>
+  <si>
+    <t>Arbeits Paket</t>
+  </si>
+  <si>
+    <t>doku</t>
+  </si>
+  <si>
+    <t>Handbuch anhand von momentanen stand anfertigen - rücksprache devs</t>
+  </si>
+  <si>
+    <t>Fertigstellung Struktur der Doku / version 1 des handbuches</t>
+  </si>
+  <si>
+    <t>aktives Schreiben der finalen Doku und des Handbuches</t>
+  </si>
+  <si>
+    <t>dev</t>
+  </si>
+  <si>
+    <t>Fertigstellung login</t>
+  </si>
+  <si>
+    <t>Fertigstellung Menü</t>
+  </si>
+  <si>
+    <t>Fertigstellung Einkaufsmodul</t>
+  </si>
+  <si>
+    <t>Fertigstellung Auswertungsmodul</t>
+  </si>
+  <si>
+    <t>Fertigstellung Gruppenverwaltungsmodul</t>
+  </si>
+  <si>
+    <t>App Fertigstellung - Pen tests</t>
+  </si>
+  <si>
+    <t>des</t>
+  </si>
+  <si>
+    <t>evaluieren aller Dokumente, die erstellt werden müssen (UMLs…)</t>
+  </si>
+  <si>
+    <t>AZ Woche - Dokumentation, Fehlerbehebung, usw</t>
+  </si>
+  <si>
+    <t>App finale Fertigstellung</t>
+  </si>
+  <si>
+    <t>Dokufertigstellung und Handbuch</t>
+  </si>
+  <si>
+    <t>Vorname</t>
+  </si>
+  <si>
+    <t>Nachname</t>
+  </si>
+  <si>
+    <t>Matrikelnummer</t>
+  </si>
+  <si>
+    <t>Mailadresse</t>
+  </si>
+  <si>
+    <t>Internal Task</t>
+  </si>
+  <si>
+    <t>Florian</t>
+  </si>
+  <si>
+    <t>Graupeter</t>
+  </si>
+  <si>
+    <t>s134213</t>
+  </si>
+  <si>
+    <t>s134213@hft-leipzig.de</t>
+  </si>
+  <si>
+    <t>Struktur und Fluss der APP</t>
+  </si>
+  <si>
+    <t>Moritz</t>
+  </si>
+  <si>
+    <t>Schaub</t>
+  </si>
+  <si>
+    <t>s134139</t>
+  </si>
+  <si>
+    <t>s134139@hft-leipzig.de</t>
+  </si>
+  <si>
+    <t>Optisches Design Der App</t>
+  </si>
+  <si>
+    <t>Karsten</t>
+  </si>
+  <si>
+    <t>s134221</t>
+  </si>
+  <si>
+    <t>s134221@hft-leipzig.de</t>
+  </si>
+  <si>
+    <t>Datenhandling und Informationsverwaltung der App</t>
+  </si>
+  <si>
+    <t>Jannis</t>
+  </si>
+  <si>
+    <t>Grohs</t>
+  </si>
+  <si>
+    <t>s134214</t>
+  </si>
+  <si>
+    <t>s134214@hft-leipzig.de</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Sawadenko</t>
+  </si>
+  <si>
+    <t>s134138</t>
+  </si>
+  <si>
+    <t>s134138@hft-leipzig.de</t>
+  </si>
+  <si>
+    <t>Eric</t>
+  </si>
+  <si>
+    <t>Sorgalla</t>
+  </si>
+  <si>
+    <t>s134146</t>
+  </si>
+  <si>
+    <t>s134146@hft-leipzig.de</t>
+  </si>
+  <si>
+    <t>Schmitt</t>
+  </si>
+  <si>
+    <t>s134141</t>
+  </si>
+  <si>
+    <t>s134141@hft-leipzig.de</t>
+  </si>
+  <si>
+    <t>Viktor</t>
+  </si>
+  <si>
+    <t>Fuchs</t>
+  </si>
+  <si>
+    <t>s134207</t>
+  </si>
+  <si>
+    <t>s134207@hft-leipzig.de</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Hein</t>
+  </si>
+  <si>
+    <t>s134248</t>
+  </si>
+  <si>
+    <t>s134248@hft-leipzig.de</t>
+  </si>
+  <si>
+    <t>Nutzerverwaltung und Back End</t>
+  </si>
+  <si>
+    <t>Sebastian</t>
+  </si>
+  <si>
+    <t>Kiepsch</t>
+  </si>
+  <si>
+    <t>s134225</t>
+  </si>
+  <si>
+    <t>s134225@hft-leipzig.de</t>
+  </si>
+  <si>
+    <t>Entwckicklungsberatung, Back End und Head Developer</t>
+  </si>
+  <si>
+    <t>Elias</t>
+  </si>
+  <si>
+    <t>s134113</t>
+  </si>
+  <si>
+    <t>Dok</t>
+  </si>
+  <si>
+    <t>s134113@hft-leipzig.de</t>
+  </si>
+  <si>
+    <t>Köstler</t>
+  </si>
+  <si>
+    <t>s134228</t>
+  </si>
+  <si>
+    <t>s134228@hft-leipzig.de</t>
+  </si>
+  <si>
+    <t>Strukturierung und Anfertiegung der Dokumentation</t>
+  </si>
+  <si>
+    <t>Dang</t>
+  </si>
+  <si>
+    <t>s134204</t>
+  </si>
+  <si>
+    <t>s134204@hft-leipzig.de</t>
+  </si>
+  <si>
+    <t>Informationssammlung und Organisation im Projekt</t>
+  </si>
+  <si>
+    <t>Markus</t>
+  </si>
+  <si>
+    <t>Hube</t>
+  </si>
+  <si>
+    <t>s134249</t>
+  </si>
+  <si>
+    <t>s134249@hft-leipzig.de</t>
+  </si>
+  <si>
+    <t>Organisation und Management des Projektes</t>
+  </si>
+  <si>
+    <t>Flexible Aufgaben und Penetrationstests (QS)</t>
+  </si>
+  <si>
+    <t>Markus und Basti</t>
+  </si>
+  <si>
+    <t>Datenbankaufbau</t>
+  </si>
+  <si>
+    <t>erneuter Abstimmungsversuch</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1771,12 +2072,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1821,8 +2116,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1847,8 +2166,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1880,12 +2205,73 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1900,11 +2286,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1913,9 +2295,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1925,55 +2304,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1995,21 +2349,104 @@
     <xf numFmtId="22" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="7" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2026,9 +2463,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2066,9 +2503,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2103,7 +2540,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2138,7 +2575,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2320,20 +2757,20 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" style="16" customWidth="1"/>
-    <col min="3" max="3" width="43.28515625" style="40" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="13" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" style="28" customWidth="1"/>
     <col min="4" max="4" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="28" t="s">
         <v>99</v>
       </c>
       <c r="D1" t="s">
@@ -2341,90 +2778,90 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="15" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="15" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="15" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="15" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="15" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="165" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="15" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="15" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="15" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2433,871 +2870,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="121.5703125" customWidth="1"/>
-    <col min="5" max="5" width="51.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" ht="225" x14ac:dyDescent="0.25">
-      <c r="A2" s="41">
-        <v>42279.657638888886</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="42">
-        <v>42283.412499999999</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="43">
-        <v>42283.412499999999</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="43">
-        <v>42283.412499999999</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="44">
-        <v>42284.313888888886</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="45">
-        <v>42284.405555555553</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="41">
-        <v>42284.418055555558</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="41">
-        <v>42287</v>
-      </c>
-      <c r="B9" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="48" customFormat="1" ht="330" x14ac:dyDescent="0.25">
-      <c r="A10" s="46">
-        <v>42287</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="E10" s="49" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="48" customFormat="1" ht="180" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" s="49" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="47">
-        <v>42289.418055555558</v>
-      </c>
-      <c r="B12" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="41">
-        <v>42290.511805555558</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="E13" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="44">
-        <v>42291.345833333333</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="44">
-        <v>42292.513888888891</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="44">
-        <v>42293.595833333333</v>
-      </c>
-      <c r="B16" t="s">
-        <v>86</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="E16" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="255" x14ac:dyDescent="0.25">
-      <c r="A17" s="44">
-        <v>42296.447222222225</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E17" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A18" s="44">
-        <v>42297.324999999997</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E18" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="44">
-        <v>42300.467361111114</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E19" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="44">
-        <v>42303.540972222225</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="G20" t="s">
-        <v>157</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="101" style="5" customWidth="1"/>
-    <col min="4" max="4" width="37.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>42283.475694444445</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>42283.484722222223</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>42283.540277777778</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>42283.627083333333</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>42283.481249999997</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>42284.464583333334</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>42285.359027777777</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="225" x14ac:dyDescent="0.25">
-      <c r="A9" s="19">
-        <v>42288</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>42300.463888888888</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="110.140625" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>42283.557638888888</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>42288</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="225" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
-        <v>42289.911805555559</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="255" x14ac:dyDescent="0.25">
-      <c r="A5" s="15">
-        <v>42292.5</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="360" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
-        <v>42288</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="C6" s="52" t="s">
-        <v>159</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C7" s="50"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="50"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="51"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="50"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="50"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="50"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="50"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="50"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="50"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="50"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="50"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="50"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="50"/>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="50"/>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="50"/>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="50"/>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" s="50"/>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C24" s="50"/>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C25" s="50"/>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C26" s="50"/>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C27" s="50"/>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C28" s="50"/>
-    </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C29" s="50"/>
-    </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C30" s="50"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D1" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
-        <v>42283.731944444444</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="37">
-        <v>42287</v>
-      </c>
-      <c r="B3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
-        <v>42292</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>42293.525694444441</v>
-      </c>
-      <c r="B5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>42296.622916666667</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D8" s="26" t="s">
-        <v>148</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="100.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="254.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="14"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="26"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3308,161 +2886,161 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+      <c r="A2" s="7">
         <v>42282.416666666664</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="7">
         <v>42282.479166666664</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="A4" s="7">
         <v>42283.416666666664</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="7">
         <v>42283.541666666664</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="7">
         <v>42284.520833333336</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="7">
         <v>42285.416666666664</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="8"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="A8" s="7">
         <v>42285.5</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="A9" s="7">
         <v>42286.375</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="10"/>
+      <c r="C9" s="8"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="A10" s="7">
         <v>42286.4375</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="8" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+      <c r="A11" s="7">
         <v>42289.375</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="A12" s="7">
         <v>42289.416666666664</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+      <c r="A13" s="7">
         <v>42292.416666666664</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="7">
         <v>42292.458333333336</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
+      <c r="A15" s="7">
         <v>42293.416666666664</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="8" t="s">
         <v>65</v>
       </c>
     </row>
@@ -3470,10 +3048,10 @@
       <c r="A16" s="1">
         <v>42296.416666666664</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3481,10 +3059,10 @@
       <c r="A17" s="1">
         <v>42297.395833333336</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="11" t="s">
         <v>124</v>
       </c>
     </row>
@@ -3492,10 +3070,10 @@
       <c r="A18" s="1">
         <v>42298.395833333336</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="11" t="s">
         <v>125</v>
       </c>
     </row>
@@ -3503,10 +3081,10 @@
       <c r="A19" s="1">
         <v>42300.375</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="11" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3514,10 +3092,10 @@
       <c r="A20" s="1">
         <v>42303.416666666664</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="11" t="s">
         <v>128</v>
       </c>
     </row>
@@ -3525,10 +3103,10 @@
       <c r="A21" s="1">
         <v>42303.458333333336</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="11" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3536,11 +3114,33 @@
       <c r="A22" s="1">
         <v>42304.395833333336</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="11" t="s">
         <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>42304.458333333336</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>42305.395833333336</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -3550,7 +3150,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -3565,25 +3165,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
+      <c r="A4" s="14">
         <v>42288</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="12" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="15" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3591,7 +3191,7 @@
       <c r="A7" s="4">
         <v>42300.470833333333</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="15" t="s">
         <v>123</v>
       </c>
     </row>
@@ -3602,4 +3202,1409 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.85546875" style="48" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="121.5703125" customWidth="1"/>
+    <col min="5" max="5" width="51.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="G1" s="51" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="225" x14ac:dyDescent="0.25">
+      <c r="A2" s="29">
+        <v>42279.657638888886</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="30">
+        <v>42283.412499999999</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="31">
+        <v>42283.412499999999</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="31">
+        <v>42283.412499999999</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="32">
+        <v>42284.313888888886</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="33">
+        <v>42284.405555555553</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="29">
+        <v>42284.418055555558</v>
+      </c>
+      <c r="B8" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="29">
+        <v>42287</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="36" customFormat="1" ht="330" x14ac:dyDescent="0.25">
+      <c r="A10" s="34">
+        <v>42287</v>
+      </c>
+      <c r="B10" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="37" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="36" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A11" s="34"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="35">
+        <v>42289.418055555558</v>
+      </c>
+      <c r="B12" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="29">
+        <v>42290.511805555558</v>
+      </c>
+      <c r="B13" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="32">
+        <v>42291.345833333333</v>
+      </c>
+      <c r="B14" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="32">
+        <v>42292.513888888891</v>
+      </c>
+      <c r="B15" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="32">
+        <v>42293.595833333333</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+      <c r="A17" s="32">
+        <v>42296.447222222225</v>
+      </c>
+      <c r="B17" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A18" s="32">
+        <v>42297.324999999997</v>
+      </c>
+      <c r="B18" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="32">
+        <v>42300.467361111114</v>
+      </c>
+      <c r="B19" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E19" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="32">
+        <v>42303.540972222225</v>
+      </c>
+      <c r="B20" s="48" t="s">
+        <v>155</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G20" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="38">
+        <v>42304</v>
+      </c>
+      <c r="B21" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:G1"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" style="48" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" style="48" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="101" style="55" customWidth="1"/>
+    <col min="4" max="4" width="37.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="57" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="51" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="52">
+        <v>42283.475694444445</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="52">
+        <v>42283.484722222223</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A4" s="52">
+        <v>42283.540277777778</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="52">
+        <v>42283.627083333333</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="52">
+        <v>42283.481249999997</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="52">
+        <v>42284.464583333334</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="52">
+        <v>42285.359027777777</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="55" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+      <c r="A9" s="56">
+        <v>42288</v>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="52">
+        <v>42300.463888888888</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="55" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F1"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="58" customWidth="1"/>
+    <col min="3" max="3" width="110.140625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="57" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="51" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>42283.557638888888</v>
+      </c>
+      <c r="B2" s="58" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>42288</v>
+      </c>
+      <c r="B3" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+      <c r="A4" s="60">
+        <v>42289.911805555559</v>
+      </c>
+      <c r="B4" s="58" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="255" x14ac:dyDescent="0.25">
+      <c r="A5" s="60">
+        <v>42292.5</v>
+      </c>
+      <c r="B5" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="59" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="360" x14ac:dyDescent="0.25">
+      <c r="A6" s="61">
+        <v>42288</v>
+      </c>
+      <c r="B6" s="58" t="s">
+        <v>158</v>
+      </c>
+      <c r="C6" s="62" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="63"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="63"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="64"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="63"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="63"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="63"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="63"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C14" s="63"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C15" s="63"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="63"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="63"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="63"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="63"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="63"/>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="63"/>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="63"/>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="63"/>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="63"/>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="63"/>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="63"/>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="63"/>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="63"/>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="63"/>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="63"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F1"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" style="56" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" style="48" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="51" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="56">
+        <v>42283.731944444444</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="56">
+        <v>42287</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="56">
+        <v>42292</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="56">
+        <v>42293.525694444441</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="56">
+        <v>42296.622916666667</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="59" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="20" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="68" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="69" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="39">
+        <v>42321</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="39">
+        <v>42328</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="39">
+        <v>42342</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="39">
+        <v>42307</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="39">
+        <v>42314</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="39">
+        <v>42321</v>
+      </c>
+      <c r="B7" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="39">
+        <v>42328</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="39">
+        <v>42335</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="C9" s="40" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="39">
+        <v>42342</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="39">
+        <v>42300</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="39">
+        <v>42314</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="C12" s="40" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="39">
+        <v>42321</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="C13" s="40" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="39">
+        <v>42328</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="39">
+        <v>42328</v>
+      </c>
+      <c r="B15" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="39">
+        <v>42342</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="40" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="39">
+        <v>42349</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="39">
+        <v>42356</v>
+      </c>
+      <c r="B18" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="40" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C1"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="11.42578125" style="8"/>
+    <col min="5" max="5" width="22" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.7109375" style="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="71" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="70" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="70" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="70" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" s="70" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="70" t="s">
+        <v>183</v>
+      </c>
+      <c r="F1" s="70" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>243</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F1"/>
+  <hyperlinks>
+    <hyperlink ref="E15" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="100.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="254.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="20"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Skillliste, Ablaufplan, Gruppenaufteilung
</commit_message>
<xml_diff>
--- a/Meetings/Doku/Struktur_Doku - 2015.10.12 - EinkaufsApp Übersicht bis dato - AK HD TE.xlsx
+++ b/Meetings/Doku/Struktur_Doku - 2015.10.12 - EinkaufsApp Übersicht bis dato - AK HD TE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="6135" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="6135"/>
   </bookViews>
   <sheets>
     <sheet name="Skilltabelle" sheetId="9" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="251">
   <si>
     <t>Datum</t>
   </si>
@@ -2045,6 +2045,13 @@
   </si>
   <si>
     <t>erneuter Abstimmungsversuch</t>
+  </si>
+  <si>
+    <t>Victor Fuchs</t>
+  </si>
+  <si>
+    <t>*gute Excelkenntnisse
+*gute Kenntnisse RW/C</t>
   </si>
 </sst>
 </file>
@@ -2749,10 +2756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2865,6 +2872,17 @@
         <v>154</v>
       </c>
     </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>250</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2875,7 +2893,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3208,7 +3226,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>

</xml_diff>

<commit_message>
Update Skillliste, Ablaufplan, Gruppenverteilung
</commit_message>
<xml_diff>
--- a/Meetings/Doku/Struktur_Doku - 2015.10.12 - EinkaufsApp Übersicht bis dato - AK HD TE.xlsx
+++ b/Meetings/Doku/Struktur_Doku - 2015.10.12 - EinkaufsApp Übersicht bis dato - AK HD TE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="6135"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="6135" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Skilltabelle" sheetId="9" r:id="rId1"/>
@@ -17,19 +17,19 @@
     <sheet name="Design" sheetId="1" r:id="rId3"/>
     <sheet name="Dev" sheetId="2" r:id="rId4"/>
     <sheet name="Doku" sheetId="7" r:id="rId5"/>
-    <sheet name="Ablaufplan" sheetId="10" r:id="rId6"/>
-    <sheet name="Gruppenaufteilung" sheetId="11" r:id="rId7"/>
+    <sheet name="Gruppenaufteilung" sheetId="11" r:id="rId6"/>
+    <sheet name="Ablaufplan" sheetId="10" r:id="rId7"/>
     <sheet name="genutzte Links" sheetId="8" r:id="rId8"/>
     <sheet name="Tools" sheetId="4" r:id="rId9"/>
     <sheet name="Telkos, Besprechungstermine" sheetId="5" r:id="rId10"/>
     <sheet name="Zusatzinfos" sheetId="6" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Ablaufplan!$A$1:$C$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">alle!$A$1:$G$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Design!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Dev!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Gruppenaufteilung!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Gruppenaufteilung!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Skilltabelle!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Telkos, Besprechungstermine'!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="251">
   <si>
     <t>Datum</t>
   </si>
@@ -1758,6 +1758,13 @@
     <t>Durchführungsphase</t>
   </si>
   <si>
+    <t>Victor Fuchs</t>
+  </si>
+  <si>
+    <t>*gute Excelkenntnisse
+*gute Kenntnisse RW/C</t>
+  </si>
+  <si>
     <t>Update</t>
   </si>
   <si>
@@ -1909,6 +1916,9 @@
     <t>s134214@hft-leipzig.de</t>
   </si>
   <si>
+    <t>Flexible Aufgaben und Penetrationstests (QS)</t>
+  </si>
+  <si>
     <t>Daniel</t>
   </si>
   <si>
@@ -2035,9 +2045,6 @@
     <t>Organisation und Management des Projektes</t>
   </si>
   <si>
-    <t>Flexible Aufgaben und Penetrationstests (QS)</t>
-  </si>
-  <si>
     <t>Markus und Basti</t>
   </si>
   <si>
@@ -2045,20 +2052,13 @@
   </si>
   <si>
     <t>erneuter Abstimmungsversuch</t>
-  </si>
-  <si>
-    <t>Victor Fuchs</t>
-  </si>
-  <si>
-    <t>*gute Excelkenntnisse
-*gute Kenntnisse RW/C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2079,6 +2079,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2213,6 +2219,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -2264,21 +2279,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2294,14 +2300,16 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2321,20 +2329,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -2356,23 +2365,40 @@
     <xf numFmtId="22" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2388,20 +2414,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2409,7 +2426,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2418,39 +2435,29 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="7" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -2758,29 +2765,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="13" customWidth="1"/>
-    <col min="3" max="3" width="43.28515625" style="28" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" style="29" customWidth="1"/>
     <col min="4" max="4" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="46" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2874,16 +2882,17 @@
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>249</v>
+        <v>161</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>108</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>250</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D1"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2892,8 +2901,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2903,162 +2913,162 @@
     <col min="3" max="3" width="43.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:3" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="72" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+      <c r="A2" s="8">
         <v>42282.416666666664</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="A3" s="8">
         <v>42282.479166666664</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="A4" s="8">
         <v>42283.416666666664</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="A5" s="8">
         <v>42283.541666666664</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="9" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="A6" s="8">
         <v>42284.520833333336</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="A7" s="8">
         <v>42285.416666666664</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="A8" s="8">
         <v>42285.5</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="9" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+      <c r="A9" s="8">
         <v>42286.375</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="8"/>
+      <c r="C9" s="9"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="8">
         <v>42286.4375</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="9" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="A11" s="8">
         <v>42289.375</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="A12" s="8">
         <v>42289.416666666664</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="9" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+      <c r="A13" s="8">
         <v>42292.416666666664</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="9" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+      <c r="A14" s="8">
         <v>42292.458333333336</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="9" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+      <c r="A15" s="8">
         <v>42293.416666666664</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="9" t="s">
         <v>65</v>
       </c>
     </row>
@@ -3066,10 +3076,10 @@
       <c r="A16" s="1">
         <v>42296.416666666664</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3077,10 +3087,10 @@
       <c r="A17" s="1">
         <v>42297.395833333336</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>124</v>
       </c>
     </row>
@@ -3088,10 +3098,10 @@
       <c r="A18" s="1">
         <v>42298.395833333336</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>125</v>
       </c>
     </row>
@@ -3099,10 +3109,10 @@
       <c r="A19" s="1">
         <v>42300.375</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="10" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3110,10 +3120,10 @@
       <c r="A20" s="1">
         <v>42303.416666666664</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>128</v>
       </c>
     </row>
@@ -3121,10 +3131,10 @@
       <c r="A21" s="1">
         <v>42303.458333333336</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3132,10 +3142,10 @@
       <c r="A22" s="1">
         <v>42304.395833333336</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="10" t="s">
         <v>131</v>
       </c>
     </row>
@@ -3143,22 +3153,22 @@
       <c r="A23" s="1">
         <v>42304.458333333336</v>
       </c>
-      <c r="B23" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>247</v>
+      <c r="B23" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>42305.395833333336</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>248</v>
+      <c r="C24" s="10" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -3196,7 +3206,7 @@
       <c r="A4" s="14">
         <v>42288</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>57</v>
       </c>
     </row>
@@ -3226,44 +3236,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.85546875" style="48" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.85546875" style="43" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="121.5703125" customWidth="1"/>
     <col min="5" max="5" width="51.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="G1" s="49" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" ht="225" x14ac:dyDescent="0.25">
-      <c r="A2" s="29">
+      <c r="A2" s="30">
         <v>42279.657638888886</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="50" t="s">
         <v>66</v>
       </c>
       <c r="C2" s="23" t="s">
@@ -3274,10 +3284,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="30">
+      <c r="A3" s="31">
         <v>42283.412499999999</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="51" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="17" t="s">
@@ -3285,10 +3295,10 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="31">
+      <c r="A4" s="32">
         <v>42283.412499999999</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="52" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="22" t="s">
@@ -3296,10 +3306,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="31">
+      <c r="A5" s="32">
         <v>42283.412499999999</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="52" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="22" t="s">
@@ -3310,10 +3320,10 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="32">
+      <c r="A6" s="33">
         <v>42284.313888888886</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="53" t="s">
         <v>67</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -3324,10 +3334,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="33">
+      <c r="A7" s="34">
         <v>42284.405555555553</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="51" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="17" t="s">
@@ -3335,10 +3345,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29">
+      <c r="A8" s="30">
         <v>42284.418055555558</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="52" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="24" t="s">
@@ -3349,10 +3359,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29">
+      <c r="A9" s="30">
         <v>42287</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="52" t="s">
         <v>61</v>
       </c>
       <c r="C9" s="25" t="s">
@@ -3362,38 +3372,38 @@
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="36" customFormat="1" ht="330" x14ac:dyDescent="0.25">
-      <c r="A10" s="34">
+    <row r="10" spans="1:7" s="37" customFormat="1" ht="330" x14ac:dyDescent="0.25">
+      <c r="A10" s="35">
         <v>42287</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="54" t="s">
         <v>63</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E10" s="38" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="36" customFormat="1" ht="180" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
-      <c r="B11" s="46"/>
+    <row r="11" spans="1:7" s="37" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A11" s="35"/>
+      <c r="B11" s="54"/>
       <c r="C11" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="37" t="s">
+      <c r="E11" s="38" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="35">
+      <c r="A12" s="36">
         <v>42289.418055555558</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="28" t="s">
         <v>72</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -3401,10 +3411,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="29">
+      <c r="A13" s="30">
         <v>42290.511805555558</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="52" t="s">
         <v>50</v>
       </c>
       <c r="C13" s="24" t="s">
@@ -3415,10 +3425,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="32">
+      <c r="A14" s="33">
         <v>42291.345833333333</v>
       </c>
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="43" t="s">
         <v>51</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -3429,10 +3439,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="32">
+      <c r="A15" s="33">
         <v>42292.513888888891</v>
       </c>
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="43" t="s">
         <v>52</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -3440,10 +3450,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32">
+      <c r="A16" s="33">
         <v>42293.595833333333</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="9" t="s">
         <v>86</v>
       </c>
       <c r="C16" s="15" t="s">
@@ -3454,10 +3464,10 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="255" x14ac:dyDescent="0.25">
-      <c r="A17" s="32">
+      <c r="A17" s="33">
         <v>42296.447222222225</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="43" t="s">
         <v>89</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -3468,10 +3478,10 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A18" s="32">
+      <c r="A18" s="33">
         <v>42297.324999999997</v>
       </c>
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="43" t="s">
         <v>93</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -3482,10 +3492,10 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="32">
+      <c r="A19" s="33">
         <v>42300.467361111114</v>
       </c>
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="43" t="s">
         <v>121</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -3496,10 +3506,10 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="32">
+      <c r="A20" s="33">
         <v>42303.540972222225</v>
       </c>
-      <c r="B20" s="48" t="s">
+      <c r="B20" s="43" t="s">
         <v>155</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -3510,14 +3520,14 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="38">
+      <c r="A21" s="42">
         <v>42304</v>
       </c>
-      <c r="B21" s="48" t="s">
-        <v>161</v>
+      <c r="B21" s="43" t="s">
+        <v>163</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -3532,48 +3542,48 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="48" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.140625" style="48" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="101" style="55" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" style="43" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" style="43" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="101" style="60" customWidth="1"/>
     <col min="4" max="4" width="37.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.42578125" style="3" customWidth="1"/>
     <col min="6" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="49" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="52">
+      <c r="A2" s="57">
         <v>42283.475694444445</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="58" t="s">
         <v>140</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -3581,13 +3591,13 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="52">
+      <c r="A3" s="57">
         <v>42283.484722222223</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="59" t="s">
         <v>56</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -3595,13 +3605,13 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A4" s="52">
+      <c r="A4" s="57">
         <v>42283.540277777778</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="58" t="s">
         <v>75</v>
       </c>
       <c r="D4" s="19" t="s">
@@ -3609,13 +3619,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="52">
+      <c r="A5" s="57">
         <v>42283.627083333333</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="58" t="s">
         <v>76</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -3623,13 +3633,13 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="52">
+      <c r="A6" s="57">
         <v>42283.481249999997</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="58" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -3637,13 +3647,13 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="52">
+      <c r="A7" s="57">
         <v>42284.464583333334</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="60" t="s">
         <v>77</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -3651,24 +3661,24 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="52">
+      <c r="A8" s="57">
         <v>42285.359027777777</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="60" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="225" x14ac:dyDescent="0.25">
-      <c r="A9" s="56">
+      <c r="A9" s="61">
         <v>42288</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="53" t="s">
+      <c r="C9" s="58" t="s">
         <v>78</v>
       </c>
       <c r="D9" s="19" t="s">
@@ -3676,13 +3686,13 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="52">
+      <c r="A10" s="57">
         <v>42300.463888888888</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="C10" s="55" t="s">
+      <c r="C10" s="60" t="s">
         <v>120</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -3702,45 +3712,45 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="58" customWidth="1"/>
-    <col min="3" max="3" width="110.140625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="110.140625" customWidth="1"/>
     <col min="4" max="4" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="62" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="62" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+      <c r="A2" s="1">
         <v>42283.557638888888</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" t="s">
         <v>79</v>
       </c>
       <c r="D2" t="s">
@@ -3748,13 +3758,13 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="A3" s="1">
         <v>42288</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="2" t="s">
         <v>80</v>
       </c>
       <c r="D3" s="19" t="s">
@@ -3762,13 +3772,13 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="225" x14ac:dyDescent="0.25">
-      <c r="A4" s="60">
+      <c r="A4" s="12">
         <v>42289.911805555559</v>
       </c>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="2" t="s">
         <v>81</v>
       </c>
       <c r="D4" s="19" t="s">
@@ -3776,13 +3786,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="255" x14ac:dyDescent="0.25">
-      <c r="A5" s="60">
+      <c r="A5" s="12">
         <v>42292.5</v>
       </c>
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D5" s="19" t="s">
@@ -3790,13 +3800,13 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="360" x14ac:dyDescent="0.25">
-      <c r="A6" s="61">
+      <c r="A6" s="14">
         <v>42288</v>
       </c>
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="C6" s="62" t="s">
+      <c r="C6" s="41" t="s">
         <v>159</v>
       </c>
       <c r="D6" s="19" t="s">
@@ -3804,76 +3814,76 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C7" s="63"/>
+      <c r="C7" s="39"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="63"/>
+      <c r="C8" s="39"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="64"/>
+      <c r="C9" s="40"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="63"/>
+      <c r="C10" s="39"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="63"/>
+      <c r="C11" s="39"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="63"/>
+      <c r="C12" s="39"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="63"/>
+      <c r="C13" s="39"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="63"/>
+      <c r="C14" s="39"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="63"/>
+      <c r="C15" s="39"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="63"/>
+      <c r="C16" s="39"/>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="63"/>
+      <c r="C17" s="39"/>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="63"/>
+      <c r="C18" s="39"/>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="63"/>
+      <c r="C19" s="39"/>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="63"/>
+      <c r="C20" s="39"/>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="63"/>
+      <c r="C21" s="39"/>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="63"/>
+      <c r="C22" s="39"/>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" s="63"/>
+      <c r="C23" s="39"/>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C24" s="63"/>
+      <c r="C24" s="39"/>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C25" s="63"/>
+      <c r="C25" s="39"/>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C26" s="63"/>
+      <c r="C26" s="39"/>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C27" s="63"/>
+      <c r="C27" s="39"/>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C28" s="63"/>
+      <c r="C28" s="39"/>
     </row>
     <row r="29" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C29" s="63"/>
+      <c r="C29" s="39"/>
     </row>
     <row r="30" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C30" s="63"/>
+      <c r="C30" s="39"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1"/>
@@ -3887,45 +3897,36 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="56" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" style="48" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="66" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="51" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="56">
+      <c r="A2" s="7">
         <v>42283.731944444444</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="19" t="s">
@@ -3933,25 +3934,25 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="56">
+      <c r="A3" s="27">
         <v>42287</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="2" t="s">
         <v>85</v>
       </c>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="56">
+      <c r="A4" s="14">
         <v>42292</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="2" t="s">
         <v>83</v>
       </c>
       <c r="D4" s="19" t="s">
@@ -3959,13 +3960,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="56">
+      <c r="A5" s="1">
         <v>42293.525694444441</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="2" t="s">
         <v>88</v>
       </c>
       <c r="D5" s="19" t="s">
@@ -3973,13 +3974,13 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="56">
+      <c r="A6" s="1">
         <v>42296.622916666667</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="2" t="s">
         <v>92</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -3998,11 +3999,320 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="11.42578125" style="9"/>
+    <col min="5" max="5" width="22" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.7109375" style="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="68" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="68" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1" s="68" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" s="68" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="68" t="s">
+        <v>185</v>
+      </c>
+      <c r="F1" s="68" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="E15" s="70" t="s">
+        <v>246</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>247</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F1"/>
+  <hyperlinks>
+    <hyperlink ref="E15" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:C1"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4013,514 +4323,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="69" t="s">
-        <v>163</v>
+      <c r="C1" s="65" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="39">
+      <c r="A2" s="66">
         <v>42321</v>
       </c>
-      <c r="B2" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="C2" s="40" t="s">
-        <v>165</v>
+      <c r="B2" s="67" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" s="67" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="39">
+      <c r="A3" s="66">
         <v>42328</v>
       </c>
-      <c r="B3" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="C3" s="40" t="s">
+      <c r="B3" s="67" t="s">
         <v>166</v>
       </c>
+      <c r="C3" s="67" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="39">
+      <c r="A4" s="66">
         <v>42342</v>
       </c>
-      <c r="B4" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>167</v>
+      <c r="B4" s="67" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4" s="67" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="39">
+      <c r="A5" s="66">
         <v>42307</v>
       </c>
-      <c r="B5" s="40" t="s">
-        <v>168</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>169</v>
+      <c r="B5" s="67" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" s="67" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="39">
+      <c r="A6" s="66">
         <v>42314</v>
       </c>
-      <c r="B6" s="40" t="s">
-        <v>168</v>
-      </c>
-      <c r="C6" s="40" t="s">
+      <c r="B6" s="67" t="s">
         <v>170</v>
       </c>
+      <c r="C6" s="67" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="39">
+      <c r="A7" s="66">
         <v>42321</v>
       </c>
-      <c r="B7" s="40" t="s">
-        <v>168</v>
-      </c>
-      <c r="C7" s="40" t="s">
+      <c r="B7" s="67" t="s">
+        <v>170</v>
+      </c>
+      <c r="C7" s="67" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="66">
+        <v>42328</v>
+      </c>
+      <c r="B8" s="67" t="s">
+        <v>170</v>
+      </c>
+      <c r="C8" s="67" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="66">
+        <v>42335</v>
+      </c>
+      <c r="B9" s="67" t="s">
+        <v>170</v>
+      </c>
+      <c r="C9" s="67" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="66">
+        <v>42342</v>
+      </c>
+      <c r="B10" s="67" t="s">
+        <v>170</v>
+      </c>
+      <c r="C10" s="67" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="66">
+        <v>42300</v>
+      </c>
+      <c r="B11" s="67" t="s">
+        <v>177</v>
+      </c>
+      <c r="C11" s="67" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="39">
+    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="66">
+        <v>42314</v>
+      </c>
+      <c r="B12" s="67" t="s">
+        <v>177</v>
+      </c>
+      <c r="C12" s="67" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="66">
+        <v>42321</v>
+      </c>
+      <c r="B13" s="67" t="s">
+        <v>177</v>
+      </c>
+      <c r="C13" s="67" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="66">
         <v>42328</v>
       </c>
-      <c r="B8" s="40" t="s">
-        <v>168</v>
-      </c>
-      <c r="C8" s="40" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="39">
-        <v>42335</v>
-      </c>
-      <c r="B9" s="40" t="s">
-        <v>168</v>
-      </c>
-      <c r="C9" s="40" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="39">
+      <c r="B14" s="67" t="s">
+        <v>177</v>
+      </c>
+      <c r="C14" s="67" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="66">
+        <v>42328</v>
+      </c>
+      <c r="B15" s="67" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="67" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="66">
         <v>42342</v>
       </c>
-      <c r="B10" s="40" t="s">
-        <v>168</v>
-      </c>
-      <c r="C10" s="40" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="39">
-        <v>42300</v>
-      </c>
-      <c r="B11" s="40" t="s">
-        <v>175</v>
-      </c>
-      <c r="C11" s="40" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="39">
-        <v>42314</v>
-      </c>
-      <c r="B12" s="40" t="s">
-        <v>175</v>
-      </c>
-      <c r="C12" s="40" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="39">
-        <v>42321</v>
-      </c>
-      <c r="B13" s="40" t="s">
-        <v>175</v>
-      </c>
-      <c r="C13" s="40" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="39">
-        <v>42328</v>
-      </c>
-      <c r="B14" s="40" t="s">
-        <v>175</v>
-      </c>
-      <c r="C14" s="40" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="39">
-        <v>42328</v>
-      </c>
-      <c r="B15" s="40" t="s">
+      <c r="B16" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="40" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="39">
-        <v>42342</v>
-      </c>
-      <c r="B16" s="40" t="s">
+      <c r="C16" s="67" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="66">
+        <v>42349</v>
+      </c>
+      <c r="B17" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="40" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="39">
-        <v>42349</v>
-      </c>
-      <c r="B17" s="40" t="s">
+      <c r="C17" s="67" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="66">
+        <v>42356</v>
+      </c>
+      <c r="B18" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="40" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="39">
-        <v>42356</v>
-      </c>
-      <c r="B18" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="40" t="s">
-        <v>179</v>
+      <c r="C18" s="67" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1"/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="4" width="11.42578125" style="8"/>
-    <col min="5" max="5" width="22" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="50.7109375" style="8" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="71" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
-        <v>180</v>
-      </c>
-      <c r="B1" s="70" t="s">
-        <v>181</v>
-      </c>
-      <c r="C1" s="70" t="s">
-        <v>182</v>
-      </c>
-      <c r="D1" s="70" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="70" t="s">
-        <v>183</v>
-      </c>
-      <c r="F1" s="70" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="E15" s="41" t="s">
-        <v>243</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>244</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:F1"/>
-  <hyperlinks>
-    <hyperlink ref="E15" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4560,7 +4560,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
-      <c r="B8" s="12"/>
+      <c r="B8" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Hinzufügen Handbuch und Update der Excel
</commit_message>
<xml_diff>
--- a/Meetings/Doku/Struktur_Doku - 2015.10.12 - EinkaufsApp Übersicht bis dato - AK HD TE.xlsx
+++ b/Meetings/Doku/Struktur_Doku - 2015.10.12 - EinkaufsApp Übersicht bis dato - AK HD TE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="6135" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="6135" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Skilltabelle" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="266">
   <si>
     <t>Datum</t>
   </si>
@@ -2115,6 +2115,11 @@
   <si>
     <t>PAP erweitert:
 Gruppeneinkauf vereinfacht, Einkauf fortsetzen eingebaut, PW rücksetzen</t>
+  </si>
+  <si>
+    <t>*Idee: Facebook, Twitter usw. zur Registrierung verwenden
+*Artikel zuweisen nach Einkauf auf Gruppenmitglieder (Noch muss gleich bei Einkau eingepflegt werden)
+*was passiert falls kein Empfang (Offline-Version)</t>
   </si>
 </sst>
 </file>
@@ -2966,7 +2971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
@@ -3267,10 +3272,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3308,6 +3313,14 @@
       </c>
       <c r="B7" s="15" t="s">
         <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>42311</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -3325,7 +3338,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Excel am 05.11.
</commit_message>
<xml_diff>
--- a/Meetings/Doku/Struktur_Doku - 2015.10.12 - EinkaufsApp Übersicht bis dato - AK HD TE.xlsx
+++ b/Meetings/Doku/Struktur_Doku - 2015.10.12 - EinkaufsApp Übersicht bis dato - AK HD TE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="6135" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="6135" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Skilltabelle" sheetId="9" r:id="rId1"/>
@@ -12,27 +12,28 @@
     <sheet name="Design" sheetId="1" r:id="rId3"/>
     <sheet name="Dev" sheetId="2" r:id="rId4"/>
     <sheet name="Doku" sheetId="7" r:id="rId5"/>
-    <sheet name="Gruppenaufteilung" sheetId="11" r:id="rId6"/>
-    <sheet name="Ablaufplan" sheetId="10" r:id="rId7"/>
-    <sheet name="genutzte Links" sheetId="8" r:id="rId8"/>
-    <sheet name="Tools" sheetId="4" r:id="rId9"/>
-    <sheet name="Telkos, Besprechungstermine" sheetId="5" r:id="rId10"/>
-    <sheet name="Zusatzinfos" sheetId="6" r:id="rId11"/>
+    <sheet name="Ideen" sheetId="12" r:id="rId6"/>
+    <sheet name="genutzte Links" sheetId="8" r:id="rId7"/>
+    <sheet name="Tools" sheetId="4" r:id="rId8"/>
+    <sheet name="Ablaufplan" sheetId="10" r:id="rId9"/>
+    <sheet name="Gruppenaufteilung" sheetId="11" r:id="rId10"/>
+    <sheet name="Telkos, Besprechungstermine" sheetId="5" r:id="rId11"/>
+    <sheet name="Zusatzinfos" sheetId="6" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">alle!$A$1:$G$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Design!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Dev!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Gruppenaufteilung!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Gruppenaufteilung!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Skilltabelle!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Telkos, Besprechungstermine'!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Telkos, Besprechungstermine'!$A$1:$C$1</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="279">
   <si>
     <t>Datum</t>
   </si>
@@ -2103,9 +2104,6 @@
     <t>unsere ToDos müssen wir in Doku mit aufnehmen aber direkte Umsetzung und bla nicht mit reinnehmen</t>
   </si>
   <si>
-    <t>ToDOs</t>
-  </si>
-  <si>
     <t>Eric Sorgalla: Bilderkennung von Preisschildern der Produkte und dann daraus EAN, Name und Preis definieren
 --&gt; hat Kontakte mit denen er dies durchführen will</t>
   </si>
@@ -2117,9 +2115,93 @@
 Gruppeneinkauf vereinfacht, Einkauf fortsetzen eingebaut, PW rücksetzen</t>
   </si>
   <si>
+    <t>Gespräch mit Frau Wieland + Herrn Georg</t>
+  </si>
+  <si>
+    <t>*Dozenten wollen GitHub Link für Repositories
+*Klassendiagramm: z.B. Kühlschrank mit Produkten und Verfallsdatum,…. --&gt; muss nur in Doku stehen!
+*Vorgehensmodell sollten wir nenen
+*Liste von Anfoderungen an App ist sehr interessant für Frau Wieland, Anforderungen struturieren nach: basic, must have, nice to have und priorisieren
+*scope: Sicherheit!! ganz wichtig und unbedingt in Doku aufnehmen
+*out of focus Anforderungen sollen auch angegebenund priorisiert werden 
+*Architektur unbedingt angeben in Doku! Multi-Tier
+*Frameworks die genutzt werden, müssen gekennzeichnet werden
+*Frau Wieland hat Qualitätsmesser für Frameworks
+*private, package,protected sind in Ordnung aber public ist nicht gut
+Infos für Präsentation:
+*20min Zeit zum präsentieren, es kann auch nur einer oder zwei votragen
+*Video vorfühen ist in Ordnung
+*Fokus der Präsentation liegt auf Frau Wieland und NICHT auf Kunde!
+Infos für Doku:
+*ca. 30 Seiten als .pdf in ilias abzugeben
+*Handbuch und Installationsanweisung muss in den Anhang
+*alles was &gt;1 Tag Verspätung hat kostet Prozente!
+Termininfo:
+*08.01.2016: Vorstellung der Präsentation- Presse wird anwesend sein; frühestes Ende um 16 Uhr</t>
+  </si>
+  <si>
+    <t>Besprechung und aktueller Stand</t>
+  </si>
+  <si>
+    <t>Gespräch mit Frau Wieland</t>
+  </si>
+  <si>
+    <t>Abspachen Handbuch</t>
+  </si>
+  <si>
+    <t>Absprachen ToDos</t>
+  </si>
+  <si>
+    <t>ToDos</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
+    <t>*Gruppenverwaltung wurde zu Verwaltung allgemein:  Verwaltung von Gruppen UND KONTAKTE 
+*Kontaktverwaltung wird noch erstellt</t>
+  </si>
+  <si>
+    <t>DB Modell überarbeitet, Arbeitspakete für jeden zugewiesen über Trello:
+Viktor Fuchs:
+Namenskonventionen ausarbeiten - Variablen und Funktionen
+Eric Sorgalla:
+Einführung in die Technik- Präsentation vorbereiten
+Modulplan erstellen
+Kanban-Board erstellen
+Florian Schmitt:
+HTML-Code der Proto.io App exportieren u. durchgehen
+Michael Hein:
+bereits erstellten Code kommentieren
+Sebastian Kiepsch:
+Einführung in die Technik- Präsentation vorbereiten
+Modulplan erstellen
+bereits erstellten Code kommentieren
+offene Aufgaben:
+*aktualisiertes DB Modell erstellen
+*EAN Kategorien recherchieren und Tabelle füllen
+*neues DB Modell implementieren
+*UML Diagramm erstellen</t>
+  </si>
+  <si>
     <t>*Idee: Facebook, Twitter usw. zur Registrierung verwenden
-*Artikel zuweisen nach Einkauf auf Gruppenmitglieder (Noch muss gleich bei Einkau eingepflegt werden)
+*Artikel zuweisen nach Einkauf auf Gruppenmitglieder (Noch muss gleich bei Einkauf eingepflegt werden)
 *was passiert falls kein Empfang (Offline-Version)</t>
+  </si>
+  <si>
+    <t>out of focus</t>
+  </si>
+  <si>
+    <t>trello</t>
+  </si>
+  <si>
+    <t>*Handbuch Inhaltsverzeichnis erstellt und Aufteilung der Aufgaben:
+Thomas: Einführung
+Huong: Einzeleinkauf (vorerst)
+Annika: Installationsanleitung</t>
+  </si>
+  <si>
+    <t>Durchführung</t>
   </si>
 </sst>
 </file>
@@ -2836,8 +2918,8 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2969,11 +3051,318 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="11.42578125" style="9"/>
+    <col min="5" max="5" width="22" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.7109375" style="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="67" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="67" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1" s="67" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" s="67" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="67" t="s">
+        <v>185</v>
+      </c>
+      <c r="F1" s="67" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="E15" t="s">
+        <v>246</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>247</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F1"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3263,6 +3652,50 @@
         <v>251</v>
       </c>
     </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>42311.583333333336</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>42312.635416666664</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>42312.75</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>42313.375</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>267</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C1"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3270,12 +3703,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3315,13 +3748,9 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>42311</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>265</v>
-      </c>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3334,11 +3763,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3630,6 +4059,20 @@
         <v>164</v>
       </c>
     </row>
+    <row r="22" spans="1:7" ht="360" x14ac:dyDescent="0.25">
+      <c r="A22" s="41">
+        <v>42313</v>
+      </c>
+      <c r="B22" s="42" t="s">
+        <v>264</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G1"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3639,17 +4082,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" style="42" customWidth="1"/>
-    <col min="2" max="2" width="39.140625" style="42" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.140625" style="42" customWidth="1"/>
     <col min="3" max="3" width="101" style="59" customWidth="1"/>
     <col min="4" max="4" width="37.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.42578125" style="3" customWidth="1"/>
@@ -3804,10 +4247,10 @@
         <v>42303</v>
       </c>
       <c r="B11" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="C11" s="57" t="s">
         <v>263</v>
-      </c>
-      <c r="C11" s="57" t="s">
-        <v>264</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>160</v>
@@ -3850,6 +4293,17 @@
       </c>
       <c r="C14" s="57" t="s">
         <v>258</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="60">
+        <v>42312</v>
+      </c>
+      <c r="B15" s="42" t="s">
+        <v>271</v>
+      </c>
+      <c r="C15" s="57" t="s">
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -3864,8 +4318,8 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="A7:D8"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3971,17 +4425,28 @@
         <v>42307</v>
       </c>
       <c r="B7" s="71" t="s">
+        <v>270</v>
+      </c>
+      <c r="C7" s="72" t="s">
         <v>261</v>
-      </c>
-      <c r="C7" s="72" t="s">
-        <v>262</v>
       </c>
       <c r="D7" s="19" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="39"/>
+    <row r="8" spans="1:6" ht="405" x14ac:dyDescent="0.25">
+      <c r="A8" s="27">
+        <v>42312</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="C8" s="72" t="s">
+        <v>273</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C9" s="40"/>
@@ -4058,10 +4523,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4176,6 +4641,20 @@
         <v>148</v>
       </c>
     </row>
+    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="27">
+        <v>42311</v>
+      </c>
+      <c r="B9" t="s">
+        <v>251</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D9" t="s">
+        <v>278</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4183,317 +4662,163 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="11.42578125" style="9"/>
-    <col min="5" max="5" width="22" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="50.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="88.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="68" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
-        <v>182</v>
-      </c>
-      <c r="B1" s="67" t="s">
-        <v>183</v>
-      </c>
-      <c r="C1" s="67" t="s">
-        <v>184</v>
-      </c>
-      <c r="D1" s="67" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="67" t="s">
-        <v>185</v>
-      </c>
-      <c r="F1" s="67" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>229</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>241</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="E15" t="s">
-        <v>246</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>247</v>
+    <row r="1" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="12">
+        <v>42311</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="60">
+        <v>42306</v>
+      </c>
+      <c r="B2" s="57" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="60">
+        <v>42306</v>
+      </c>
+      <c r="B3" s="57" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="100.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="254.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="20"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>276</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4704,106 +5029,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="100.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="254.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="11"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="20"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Ergänzung Skilliste von Thomas
</commit_message>
<xml_diff>
--- a/Meetings/Doku/Struktur_Doku - 2015.10.12 - EinkaufsApp Übersicht bis dato - AK HD TE.xlsx
+++ b/Meetings/Doku/Struktur_Doku - 2015.10.12 - EinkaufsApp Übersicht bis dato - AK HD TE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="6135" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="6135" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Skilltabelle" sheetId="9" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="287">
   <si>
     <t>Datum</t>
   </si>
@@ -2217,6 +2217,24 @@
   </si>
   <si>
     <t>wird noch nicht implementiert</t>
+  </si>
+  <si>
+    <t>Thomas Elias</t>
+  </si>
+  <si>
+    <t>* gute Kenntnisse in Projektkoordination
+* Anforderungen und Arbeitspakete definieren
+* Erfahrungen Customizing von Dokumenten-Layouts
+* Kommunikation zwischen versch. Abteilungen zum Transparent-Machen der Informationen</t>
+  </si>
+  <si>
+    <t>* Diagramme erstellen (Use Cases, Activities,…</t>
+  </si>
+  <si>
+    <t>Leitung Entwicklerteam</t>
+  </si>
+  <si>
+    <t>Organisation des Projektes und Dokumentation</t>
   </si>
 </sst>
 </file>
@@ -2930,11 +2948,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="A1:D10"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3058,6 +3076,20 @@
         <v>162</v>
       </c>
     </row>
+    <row r="11" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>283</v>
+      </c>
+      <c r="D11" t="s">
+        <v>284</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D1"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3070,7 +3102,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3196,6 +3228,9 @@
       <c r="E6" s="9" t="s">
         <v>209</v>
       </c>
+      <c r="F6" s="9" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -3213,6 +3248,9 @@
       <c r="E7" s="9" t="s">
         <v>213</v>
       </c>
+      <c r="F7" s="9" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -3303,6 +3341,9 @@
       </c>
       <c r="E12" s="9" t="s">
         <v>234</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -4099,7 +4140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
@@ -4781,7 +4822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>

</xml_diff>